<commit_message>
Web scraper and file output now can handle multiple website in a single run.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>meal_category</t>
+          <t>meal-category</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -469,6 +469,28 @@
       <c r="D2" t="inlineStr">
         <is>
           <t>['4 tablespoons butter', '2 teaspoons olive oil', '1 ½ teaspoons garlic powder', 'salt and ground black pepper to taste', '6 medium potatoes, scrubbed']</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>ingredient</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://www.allrecipes.com/recipe/270750/simple-baked-potato/</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>side-dish</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['1 pound baby carrots', '1 1/2 pounds baby red potatoes, scrubbed and halved', '1/4 cup olive oil', '2 teaspoons minced fresh sage', '2 teaspoons minced fresh rosemary', '2 teaspoons minced fresh thyme', '1 teaspoon salt or to taste', '1/2 teaspoon freshly ground black pepper or to taste', '1 tablespoon minced fresh garlic or to taste', '1 onion, cut into eighths', '1 pound zucchini, halved lengthwise and cut into 1-inch pieces', '1/2 pound mushrooms, cleaned and quatered', '1 tablespoon minced fresh parsley, for garnish']</t>
         </is>
       </c>
     </row>

</xml_diff>